<commit_message>
Added very initial version of the graph builder, added functions for pdf document loading
</commit_message>
<xml_diff>
--- a/docs/Project_Workload.xlsx
+++ b/docs/Project_Workload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/souravtiwari_arizona_edu/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gagan/Projects/info_698/info-698-hybrid-rag/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{6AACE851-1339-49BA-B20A-285556F193F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79F8DC8F-71A9-40FD-8438-768E2E062B54}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDEE05D-7FEC-B541-B170-23B5E9A05022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="800" windowWidth="41120" windowHeight="24240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project schedule (Gantt Chart)" sheetId="11" r:id="rId1"/>
@@ -370,7 +370,7 @@
     <numFmt numFmtId="166" formatCode="mmm\ d\,\ yyyy"/>
     <numFmt numFmtId="167" formatCode="d"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1787,24 +1787,24 @@
   </sheetPr>
   <dimension ref="A1:BL41"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRuler="0" zoomScale="28" zoomScaleNormal="39" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="AT11" sqref="AT11"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A14" zoomScale="150" zoomScaleNormal="39" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="73.125" customWidth="1"/>
-    <col min="3" max="3" width="16.625" customWidth="1"/>
-    <col min="4" max="4" width="10.625" customWidth="1"/>
-    <col min="5" max="5" width="10.625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.625" customWidth="1"/>
-    <col min="7" max="7" width="2.625" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="73.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="2.6640625" customWidth="1"/>
     <col min="8" max="8" width="6" hidden="1" customWidth="1"/>
-    <col min="9" max="65" width="2.625" customWidth="1"/>
+    <col min="9" max="65" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="60.95">
+    <row r="1" spans="1:64" ht="64" x14ac:dyDescent="0.4">
       <c r="A1" s="5"/>
       <c r="B1" s="105" t="s">
         <v>0</v>
@@ -1841,7 +1841,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:64" ht="30" customHeight="1">
+    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="67" t="s">
         <v>3</v>
       </c>
@@ -1874,13 +1874,13 @@
       <c r="Y2" s="116"/>
       <c r="Z2" s="116"/>
     </row>
-    <row r="3" spans="1:64" s="15" customFormat="1" ht="30" customHeight="1">
+    <row r="3" spans="1:64" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4"/>
       <c r="B3" s="14"/>
       <c r="D3" s="16"/>
       <c r="E3" s="17"/>
     </row>
-    <row r="4" spans="1:64" s="15" customFormat="1" ht="30" customHeight="1">
+    <row r="4" spans="1:64" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5"/>
       <c r="B4" s="18"/>
       <c r="E4" s="19"/>
@@ -1965,7 +1965,7 @@
       <c r="BK4" s="120"/>
       <c r="BL4" s="120"/>
     </row>
-    <row r="5" spans="1:64" s="15" customFormat="1" ht="15" customHeight="1">
+    <row r="5" spans="1:64" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="115"/>
       <c r="B5" s="113" t="s">
         <v>6</v>
@@ -2207,7 +2207,7 @@
         <v>45991</v>
       </c>
     </row>
-    <row r="6" spans="1:64" s="15" customFormat="1" ht="15" customHeight="1" thickBot="1">
+    <row r="6" spans="1:64" s="15" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="115"/>
       <c r="B6" s="114"/>
       <c r="C6" s="112"/>
@@ -2439,7 +2439,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="7" spans="1:64" s="15" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
+    <row r="7" spans="1:64" s="15" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
@@ -2449,7 +2449,7 @@
       <c r="E7" s="26"/>
       <c r="F7" s="26"/>
       <c r="H7" s="15" t="str">
-        <f ca="1">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I7" s="28"/>
@@ -2509,7 +2509,7 @@
       <c r="BK7" s="28"/>
       <c r="BL7" s="28"/>
     </row>
-    <row r="8" spans="1:64" s="33" customFormat="1" ht="60.95" customHeight="1" thickBot="1">
+    <row r="8" spans="1:64" s="33" customFormat="1" ht="61" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="29" t="s">
         <v>12</v>
@@ -2530,7 +2530,7 @@
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="3">
-        <f t="shared" ref="H8:H41" ca="1" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H41" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v>8</v>
       </c>
       <c r="I8" s="34"/>
@@ -2590,7 +2590,7 @@
       <c r="BK8" s="34"/>
       <c r="BL8" s="34"/>
     </row>
-    <row r="9" spans="1:64" s="33" customFormat="1" ht="56.45" customHeight="1" thickBot="1">
+    <row r="9" spans="1:64" s="33" customFormat="1" ht="56.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="29" t="s">
         <v>14</v>
@@ -2611,7 +2611,7 @@
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="3">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="I9" s="34"/>
@@ -2671,7 +2671,7 @@
       <c r="BK9" s="34"/>
       <c r="BL9" s="34"/>
     </row>
-    <row r="10" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="10" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="29" t="s">
         <v>16</v>
@@ -2679,7 +2679,9 @@
       <c r="C10" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="30"/>
+      <c r="D10" s="30">
+        <v>1</v>
+      </c>
       <c r="E10" s="31">
         <f>F9</f>
         <v>45929</v>
@@ -2690,7 +2692,7 @@
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="3">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="I10" s="34"/>
@@ -2750,7 +2752,7 @@
       <c r="BK10" s="34"/>
       <c r="BL10" s="34"/>
     </row>
-    <row r="11" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="11" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="71" t="s">
         <v>18</v>
@@ -2761,7 +2763,7 @@
       <c r="F11" s="75"/>
       <c r="G11" s="6"/>
       <c r="H11" s="3" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I11" s="34"/>
@@ -2821,7 +2823,7 @@
       <c r="BK11" s="34"/>
       <c r="BL11" s="34"/>
     </row>
-    <row r="12" spans="1:64" s="33" customFormat="1" ht="50.45" thickBot="1">
+    <row r="12" spans="1:64" s="33" customFormat="1" ht="57" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="35" t="s">
         <v>19</v>
@@ -2829,7 +2831,9 @@
       <c r="C12" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="37"/>
+      <c r="D12" s="37">
+        <v>1</v>
+      </c>
       <c r="E12" s="38">
         <f>DATE(2025,10,10)</f>
         <v>45940</v>
@@ -2897,7 +2901,7 @@
       <c r="BK12" s="34"/>
       <c r="BL12" s="34"/>
     </row>
-    <row r="13" spans="1:64" s="33" customFormat="1" ht="50.45" thickBot="1">
+    <row r="13" spans="1:64" s="33" customFormat="1" ht="57" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="35" t="s">
         <v>20</v>
@@ -2905,7 +2909,9 @@
       <c r="C13" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="37"/>
+      <c r="D13" s="37">
+        <v>1</v>
+      </c>
       <c r="E13" s="38">
         <f>E12</f>
         <v>45940</v>
@@ -2973,7 +2979,7 @@
       <c r="BK13" s="34"/>
       <c r="BL13" s="34"/>
     </row>
-    <row r="14" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="14" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="35" t="s">
         <v>21</v>
@@ -2981,7 +2987,9 @@
       <c r="C14" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="37"/>
+      <c r="D14" s="37">
+        <v>1</v>
+      </c>
       <c r="E14" s="38">
         <f>E13</f>
         <v>45940</v>
@@ -3049,7 +3057,7 @@
       <c r="BK14" s="34"/>
       <c r="BL14" s="34"/>
     </row>
-    <row r="15" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="15" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="35" t="s">
         <v>22</v>
@@ -3057,7 +3065,9 @@
       <c r="C15" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="37"/>
+      <c r="D15" s="37">
+        <v>1</v>
+      </c>
       <c r="E15" s="38">
         <f>E14</f>
         <v>45940</v>
@@ -3068,7 +3078,7 @@
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="3">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="I15" s="34"/>
@@ -3128,7 +3138,7 @@
       <c r="BK15" s="34"/>
       <c r="BL15" s="34"/>
     </row>
-    <row r="16" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="16" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="40" t="s">
         <v>23</v>
@@ -3139,7 +3149,7 @@
       <c r="F16" s="44"/>
       <c r="G16" s="6"/>
       <c r="H16" s="3" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I16" s="34"/>
@@ -3199,7 +3209,7 @@
       <c r="BK16" s="34"/>
       <c r="BL16" s="34"/>
     </row>
-    <row r="17" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="17" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="45" t="s">
         <v>24</v>
@@ -3207,7 +3217,9 @@
       <c r="C17" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="47"/>
+      <c r="D17" s="47">
+        <v>1</v>
+      </c>
       <c r="E17" s="48">
         <f>F15</f>
         <v>45947</v>
@@ -3218,7 +3230,7 @@
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="3">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="I17" s="34"/>
@@ -3278,7 +3290,7 @@
       <c r="BK17" s="34"/>
       <c r="BL17" s="34"/>
     </row>
-    <row r="18" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="18" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="45" t="s">
         <v>26</v>
@@ -3286,7 +3298,9 @@
       <c r="C18" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="47"/>
+      <c r="D18" s="47">
+        <v>1</v>
+      </c>
       <c r="E18" s="48">
         <f>E17</f>
         <v>45947</v>
@@ -3297,7 +3311,7 @@
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="3">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="I18" s="34"/>
@@ -3357,7 +3371,7 @@
       <c r="BK18" s="34"/>
       <c r="BL18" s="34"/>
     </row>
-    <row r="19" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="19" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="45" t="s">
         <v>27</v>
@@ -3365,7 +3379,9 @@
       <c r="C19" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="47"/>
+      <c r="D19" s="47">
+        <v>0.8</v>
+      </c>
       <c r="E19" s="48">
         <f>E18</f>
         <v>45947</v>
@@ -3376,7 +3392,7 @@
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="3">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="I19" s="34"/>
@@ -3436,7 +3452,7 @@
       <c r="BK19" s="34"/>
       <c r="BL19" s="34"/>
     </row>
-    <row r="20" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="20" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="49" t="s">
         <v>28</v>
@@ -3447,7 +3463,7 @@
       <c r="F20" s="53"/>
       <c r="G20" s="6"/>
       <c r="H20" s="3" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I20" s="34"/>
@@ -3507,7 +3523,7 @@
       <c r="BK20" s="34"/>
       <c r="BL20" s="34"/>
     </row>
-    <row r="21" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="21" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="54" t="s">
         <v>29</v>
@@ -3526,7 +3542,7 @@
       </c>
       <c r="G21" s="6"/>
       <c r="H21" s="3">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="I21" s="34"/>
@@ -3586,7 +3602,7 @@
       <c r="BK21" s="34"/>
       <c r="BL21" s="34"/>
     </row>
-    <row r="22" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="22" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="54" t="s">
         <v>30</v>
@@ -3605,7 +3621,7 @@
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="3">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="I22" s="34"/>
@@ -3665,7 +3681,7 @@
       <c r="BK22" s="34"/>
       <c r="BL22" s="34"/>
     </row>
-    <row r="23" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="23" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="58" t="s">
         <v>31</v>
@@ -3676,7 +3692,7 @@
       <c r="F23" s="62"/>
       <c r="G23" s="6"/>
       <c r="H23" s="3" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I23" s="34"/>
@@ -3736,7 +3752,7 @@
       <c r="BK23" s="34"/>
       <c r="BL23" s="34"/>
     </row>
-    <row r="24" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="24" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="63" t="s">
         <v>32</v>
@@ -3755,7 +3771,7 @@
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="3">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="I24" s="34"/>
@@ -3815,7 +3831,7 @@
       <c r="BK24" s="34"/>
       <c r="BL24" s="34"/>
     </row>
-    <row r="25" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="25" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="63" t="s">
         <v>34</v>
@@ -3834,7 +3850,7 @@
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="3">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="I25" s="34"/>
@@ -3894,7 +3910,7 @@
       <c r="BK25" s="34"/>
       <c r="BL25" s="34"/>
     </row>
-    <row r="26" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="26" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="63" t="s">
         <v>35</v>
@@ -3913,7 +3929,7 @@
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="3">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="I26" s="34"/>
@@ -3973,7 +3989,7 @@
       <c r="BK26" s="34"/>
       <c r="BL26" s="34"/>
     </row>
-    <row r="27" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="27" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="77" t="s">
         <v>36</v>
@@ -3984,7 +4000,7 @@
       <c r="F27" s="81"/>
       <c r="G27" s="6"/>
       <c r="H27" s="3" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I27" s="34"/>
@@ -4044,7 +4060,7 @@
       <c r="BK27" s="34"/>
       <c r="BL27" s="34"/>
     </row>
-    <row r="28" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="28" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="82" t="s">
         <v>37</v>
@@ -4063,7 +4079,7 @@
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="3">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="I28" s="34"/>
@@ -4123,7 +4139,7 @@
       <c r="BK28" s="34"/>
       <c r="BL28" s="34"/>
     </row>
-    <row r="29" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="29" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
       <c r="B29" s="82" t="s">
         <v>38</v>
@@ -4142,7 +4158,7 @@
       </c>
       <c r="G29" s="6"/>
       <c r="H29" s="3">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="I29" s="34"/>
@@ -4202,7 +4218,7 @@
       <c r="BK29" s="34"/>
       <c r="BL29" s="34"/>
     </row>
-    <row r="30" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="30" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="86" t="s">
         <v>39</v>
@@ -4213,7 +4229,7 @@
       <c r="F30" s="90"/>
       <c r="G30" s="6"/>
       <c r="H30" s="3" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I30" s="34"/>
@@ -4273,7 +4289,7 @@
       <c r="BK30" s="34"/>
       <c r="BL30" s="34"/>
     </row>
-    <row r="31" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="31" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="91" t="s">
         <v>40</v>
@@ -4292,7 +4308,7 @@
       </c>
       <c r="G31" s="6"/>
       <c r="H31" s="3">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="I31" s="34"/>
@@ -4352,7 +4368,7 @@
       <c r="BK31" s="34"/>
       <c r="BL31" s="34"/>
     </row>
-    <row r="32" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="32" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="91" t="s">
         <v>41</v>
@@ -4371,7 +4387,7 @@
       </c>
       <c r="G32" s="6"/>
       <c r="H32" s="3">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="I32" s="34"/>
@@ -4431,7 +4447,7 @@
       <c r="BK32" s="34"/>
       <c r="BL32" s="34"/>
     </row>
-    <row r="33" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="33" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="95" t="s">
         <v>42</v>
@@ -4442,7 +4458,7 @@
       <c r="F33" s="99"/>
       <c r="G33" s="6"/>
       <c r="H33" s="3" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I33" s="34"/>
@@ -4502,7 +4518,7 @@
       <c r="BK33" s="34"/>
       <c r="BL33" s="34"/>
     </row>
-    <row r="34" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="34" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="100" t="s">
         <v>43</v>
@@ -4521,7 +4537,7 @@
       </c>
       <c r="G34" s="6"/>
       <c r="H34" s="3">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="I34" s="34"/>
@@ -4581,7 +4597,7 @@
       <c r="BK34" s="34"/>
       <c r="BL34" s="34"/>
     </row>
-    <row r="35" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="35" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="100" t="s">
         <v>44</v>
@@ -4600,7 +4616,7 @@
       </c>
       <c r="G35" s="6"/>
       <c r="H35" s="3">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="I35" s="34"/>
@@ -4660,7 +4676,7 @@
       <c r="BK35" s="34"/>
       <c r="BL35" s="34"/>
     </row>
-    <row r="36" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="36" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="100" t="s">
         <v>45</v>
@@ -4679,7 +4695,7 @@
       </c>
       <c r="G36" s="6"/>
       <c r="H36" s="3">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="I36" s="34"/>
@@ -4739,7 +4755,7 @@
       <c r="BK36" s="34"/>
       <c r="BL36" s="34"/>
     </row>
-    <row r="37" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="37" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="100" t="s">
         <v>46</v>
@@ -4758,7 +4774,7 @@
       </c>
       <c r="G37" s="6"/>
       <c r="H37" s="3">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="I37" s="34"/>
@@ -4818,7 +4834,7 @@
       <c r="BK37" s="34"/>
       <c r="BL37" s="34"/>
     </row>
-    <row r="38" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="38" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="58" t="s">
         <v>47</v>
@@ -4829,7 +4845,7 @@
       <c r="F38" s="62"/>
       <c r="G38" s="6"/>
       <c r="H38" s="3" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I38" s="34"/>
@@ -4889,7 +4905,7 @@
       <c r="BK38" s="34"/>
       <c r="BL38" s="34"/>
     </row>
-    <row r="39" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="39" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="B39" s="63" t="s">
         <v>48</v>
@@ -4908,7 +4924,7 @@
       </c>
       <c r="G39" s="6"/>
       <c r="H39" s="3">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="I39" s="34"/>
@@ -4968,7 +4984,7 @@
       <c r="BK39" s="34"/>
       <c r="BL39" s="34"/>
     </row>
-    <row r="40" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="40" spans="1:64" s="33" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
       <c r="B40" s="86" t="s">
         <v>49</v>
@@ -4979,7 +4995,7 @@
       <c r="F40" s="90"/>
       <c r="G40" s="6"/>
       <c r="H40" s="3" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I40" s="34"/>
@@ -5039,7 +5055,7 @@
       <c r="BK40" s="34"/>
       <c r="BL40" s="34"/>
     </row>
-    <row r="41" spans="1:64" s="33" customFormat="1" ht="50.45" thickBot="1">
+    <row r="41" spans="1:64" s="33" customFormat="1" ht="57" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" s="91" t="s">
         <v>50</v>
@@ -5058,7 +5074,7 @@
       </c>
       <c r="G41" s="6"/>
       <c r="H41" s="3">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I41" s="34"/>
@@ -5237,25 +5253,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C9993AE-EA08-4E32-AE69-4AB3B4D0781D}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.25" customWidth="1"/>
-    <col min="3" max="3" width="21.875" customWidth="1"/>
-    <col min="4" max="4" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.625" customWidth="1"/>
-    <col min="6" max="6" width="9.625" customWidth="1"/>
-    <col min="7" max="7" width="9.25" customWidth="1"/>
-    <col min="8" max="8" width="9.125" customWidth="1"/>
-    <col min="9" max="9" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" customWidth="1"/>
+    <col min="4" max="4" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" customWidth="1"/>
+    <col min="7" max="8" width="9.1640625" customWidth="1"/>
+    <col min="9" max="9" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27.95">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.15">
       <c r="A1" s="106" t="s">
         <v>51</v>
       </c>
@@ -5284,7 +5299,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="98.1">
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.15">
       <c r="A2" s="107" t="s">
         <v>56</v>
       </c>
@@ -5313,7 +5328,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="111.95">
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.15">
       <c r="A3" s="107" t="s">
         <v>56</v>
       </c>
@@ -5342,7 +5357,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="98.1">
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.15">
       <c r="A4" s="107" t="s">
         <v>56</v>
       </c>
@@ -5365,7 +5380,7 @@
       <c r="H4" s="107"/>
       <c r="I4" s="107"/>
     </row>
-    <row r="5" spans="1:9" ht="84">
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.15">
       <c r="A5" s="107" t="s">
         <v>56</v>
       </c>
@@ -5388,7 +5403,7 @@
       <c r="H5" s="107"/>
       <c r="I5" s="107"/>
     </row>
-    <row r="6" spans="1:9" ht="56.1">
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.15">
       <c r="A6" s="107" t="s">
         <v>62</v>
       </c>
@@ -5411,7 +5426,7 @@
       <c r="H6" s="107"/>
       <c r="I6" s="107"/>
     </row>
-    <row r="7" spans="1:9" ht="69.95">
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.15">
       <c r="A7" s="107" t="s">
         <v>62</v>
       </c>
@@ -5434,7 +5449,7 @@
       </c>
       <c r="I7" s="107"/>
     </row>
-    <row r="8" spans="1:9" ht="56.1">
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.15">
       <c r="A8" s="107" t="s">
         <v>62</v>
       </c>
@@ -5457,7 +5472,7 @@
       </c>
       <c r="I8" s="107"/>
     </row>
-    <row r="9" spans="1:9" ht="111.95">
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.15">
       <c r="A9" s="107" t="s">
         <v>67</v>
       </c>
@@ -5480,7 +5495,7 @@
       <c r="H9" s="107"/>
       <c r="I9" s="107"/>
     </row>
-    <row r="10" spans="1:9" ht="69.95">
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.15">
       <c r="A10" s="107" t="s">
         <v>67</v>
       </c>
@@ -5503,7 +5518,7 @@
       </c>
       <c r="I10" s="107"/>
     </row>
-    <row r="11" spans="1:9" ht="84">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.15">
       <c r="A11" s="107" t="s">
         <v>72</v>
       </c>
@@ -5526,7 +5541,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="98.1">
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.15">
       <c r="A12" s="107" t="s">
         <v>72</v>
       </c>
@@ -5549,7 +5564,7 @@
       <c r="H12" s="107"/>
       <c r="I12" s="107"/>
     </row>
-    <row r="13" spans="1:9" ht="69.95">
+    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.15">
       <c r="A13" s="107" t="s">
         <v>72</v>
       </c>
@@ -5572,7 +5587,7 @@
       <c r="H13" s="107"/>
       <c r="I13" s="107"/>
     </row>
-    <row r="14" spans="1:9" ht="153.94999999999999">
+    <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.15">
       <c r="A14" s="107" t="s">
         <v>78</v>
       </c>
@@ -5595,7 +5610,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="69.95">
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.15">
       <c r="A15" s="107" t="s">
         <v>78</v>
       </c>
@@ -5618,7 +5633,7 @@
       <c r="H15" s="107"/>
       <c r="I15" s="107"/>
     </row>
-    <row r="16" spans="1:9" ht="111.95">
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.15">
       <c r="A16" s="107" t="s">
         <v>84</v>
       </c>
@@ -5641,7 +5656,7 @@
       <c r="H16" s="107"/>
       <c r="I16" s="107"/>
     </row>
-    <row r="17" spans="1:9" ht="84">
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.15">
       <c r="A17" s="107" t="s">
         <v>84</v>
       </c>
@@ -5664,7 +5679,7 @@
       </c>
       <c r="I17" s="107"/>
     </row>
-    <row r="18" spans="1:9" ht="69.95">
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.15">
       <c r="A18" s="107" t="s">
         <v>89</v>
       </c>
@@ -5687,7 +5702,7 @@
       <c r="H18" s="107"/>
       <c r="I18" s="107"/>
     </row>
-    <row r="19" spans="1:9" ht="69.95">
+    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.15">
       <c r="A19" s="107" t="s">
         <v>89</v>
       </c>
@@ -5710,7 +5725,7 @@
       <c r="H19" s="107"/>
       <c r="I19" s="107"/>
     </row>
-    <row r="20" spans="1:9" ht="84">
+    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.15">
       <c r="A20" s="107" t="s">
         <v>89</v>
       </c>
@@ -5733,7 +5748,7 @@
       <c r="H20" s="107"/>
       <c r="I20" s="107"/>
     </row>
-    <row r="21" spans="1:9" ht="69.95">
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.15">
       <c r="A21" s="107" t="s">
         <v>89</v>
       </c>
@@ -5756,7 +5771,7 @@
       </c>
       <c r="I21" s="107"/>
     </row>
-    <row r="22" spans="1:9" ht="98.1">
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.15">
       <c r="A22" s="107" t="s">
         <v>89</v>
       </c>
@@ -5779,7 +5794,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="56.1">
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.15">
       <c r="A23" s="107" t="s">
         <v>89</v>
       </c>
@@ -5814,15 +5829,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006B8B2E08FBA2934085025AE2CC2D4FCF" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8d5915535425329bcbd771e38b5089a6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d9b4d3a9-89d7-4752-9f66-1c4049782483" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a4a6479488fcfa1ea26509531871ed87" ns3:_="">
     <xsd:import namespace="d9b4d3a9-89d7-4752-9f66-1c4049782483"/>
@@ -5972,22 +5978,54 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E186200E-CA11-482F-967A-1FD62478FEA5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d9b4d3a9-89d7-4752-9f66-1c4049782483"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E186200E-CA11-482F-967A-1FD62478FEA5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>